<commit_message>
Modified excel sheet,feature files also handled exception
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/101-RBI-EPP-DB-DL-REC-NOCOM-RNI-CTPD-SAR-MD-TR-1-ONTIME-Newcreateloan.xlsx
+++ b/Mifos Automation Excels/Client/101-RBI-EPP-DB-DL-REC-NOCOM-RNI-CTPD-SAR-MD-TR-1-ONTIME-Newcreateloan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="495" windowWidth="15015" windowHeight="7620"/>
+    <workbookView xWindow="180" yWindow="495" windowWidth="15015" windowHeight="7620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NewLoanInput" sheetId="9" r:id="rId1"/>
@@ -148,7 +148,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -162,11 +162,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -207,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -224,9 +219,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -541,7 +533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -563,7 +555,7 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>41</v>
       </c>
     </row>
@@ -679,10 +671,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -695,7 +687,7 @@
     <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -715,8 +707,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="11">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="10">
         <v>10000</v>
       </c>
       <c r="B2" s="5">
@@ -726,15 +718,14 @@
       <c r="D2" s="5">
         <v>0</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="10">
         <v>10000</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="11">
         <v>1666.66</v>
       </c>
-      <c r="H2" s="9"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>672.06</v>
       </c>
@@ -754,7 +745,7 @@
         <v>193.97</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>0</v>
       </c>
@@ -774,7 +765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>0</v>
       </c>
@@ -804,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -881,13 +872,13 @@
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="13">
+      <c r="C2" s="12">
         <v>42005</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="11">
+      <c r="G2" s="10">
         <v>10000</v>
       </c>
       <c r="H2" s="5"/>
@@ -912,7 +903,7 @@
       <c r="B3" s="5">
         <v>31</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="12">
         <v>42036</v>
       </c>
       <c r="D3" s="5"/>
@@ -920,7 +911,7 @@
       <c r="F3" s="5">
         <v>833.33</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="11">
         <v>9166.67</v>
       </c>
       <c r="H3" s="5">
@@ -955,7 +946,7 @@
       <c r="B4" s="5">
         <v>28</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="12">
         <v>42064</v>
       </c>
       <c r="D4" s="5"/>
@@ -963,7 +954,7 @@
       <c r="F4" s="5">
         <v>833.33</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="11">
         <v>8333.34</v>
       </c>
       <c r="H4" s="5">
@@ -998,7 +989,7 @@
       <c r="B5" s="5">
         <v>31</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="12">
         <v>42095</v>
       </c>
       <c r="D5" s="5"/>
@@ -1006,7 +997,7 @@
       <c r="F5" s="5">
         <v>833.33</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="11">
         <v>7500.01</v>
       </c>
       <c r="H5" s="5">
@@ -1041,7 +1032,7 @@
       <c r="B6" s="5">
         <v>30</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="12">
         <v>42125</v>
       </c>
       <c r="D6" s="5"/>
@@ -1049,7 +1040,7 @@
       <c r="F6" s="5">
         <v>833.33</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="11">
         <v>6666.68</v>
       </c>
       <c r="H6" s="5">
@@ -1084,7 +1075,7 @@
       <c r="B7" s="5">
         <v>31</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="12">
         <v>42156</v>
       </c>
       <c r="D7" s="5"/>
@@ -1092,7 +1083,7 @@
       <c r="F7" s="5">
         <v>833.33</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="11">
         <v>5833.35</v>
       </c>
       <c r="H7" s="5">
@@ -1127,7 +1118,7 @@
       <c r="B8" s="5">
         <v>30</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="12">
         <v>42186</v>
       </c>
       <c r="D8" s="5"/>
@@ -1135,7 +1126,7 @@
       <c r="F8" s="5">
         <v>833.33</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="11">
         <v>5000.0200000000004</v>
       </c>
       <c r="H8" s="5">
@@ -1170,7 +1161,7 @@
       <c r="B9" s="5">
         <v>31</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="12">
         <v>42217</v>
       </c>
       <c r="D9" s="5"/>
@@ -1178,7 +1169,7 @@
       <c r="F9" s="5">
         <v>833.33</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="11">
         <v>4166.6899999999996</v>
       </c>
       <c r="H9" s="5">
@@ -1213,7 +1204,7 @@
       <c r="B10" s="5">
         <v>31</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="12">
         <v>42248</v>
       </c>
       <c r="D10" s="5"/>
@@ -1221,7 +1212,7 @@
       <c r="F10" s="5">
         <v>833.33</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="11">
         <v>3333.36</v>
       </c>
       <c r="H10" s="5">
@@ -1256,7 +1247,7 @@
       <c r="B11" s="5">
         <v>30</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="12">
         <v>42278</v>
       </c>
       <c r="D11" s="5"/>
@@ -1264,7 +1255,7 @@
       <c r="F11" s="5">
         <v>833.33</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="11">
         <v>2500.0300000000002</v>
       </c>
       <c r="H11" s="5">
@@ -1299,7 +1290,7 @@
       <c r="B12" s="5">
         <v>31</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="12">
         <v>42309</v>
       </c>
       <c r="D12" s="5"/>
@@ -1307,7 +1298,7 @@
       <c r="F12" s="5">
         <v>833.33</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="11">
         <v>1666.7</v>
       </c>
       <c r="H12" s="5">
@@ -1342,7 +1333,7 @@
       <c r="B13" s="5">
         <v>30</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="12">
         <v>42339</v>
       </c>
       <c r="D13" s="5"/>
@@ -1385,7 +1376,7 @@
       <c r="B14" s="5">
         <v>31</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="12">
         <v>42370</v>
       </c>
       <c r="D14" s="5"/>

</xml_diff>

<commit_message>
modified excelsheet feature files
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/101-RBI-EPP-DB-DL-REC-NOCOM-RNI-CTPD-SAR-MD-TR-1-ONTIME-Newcreateloan.xlsx
+++ b/Mifos Automation Excels/Client/101-RBI-EPP-DB-DL-REC-NOCOM-RNI-CTPD-SAR-MD-TR-1-ONTIME-Newcreateloan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="495" windowWidth="15015" windowHeight="7620"/>
+    <workbookView xWindow="180" yWindow="495" windowWidth="15015" windowHeight="7620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NewLoanInput" sheetId="9" r:id="rId1"/>
@@ -148,7 +148,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -162,11 +162,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -207,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -224,9 +219,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -541,7 +533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -563,7 +555,7 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>41</v>
       </c>
     </row>
@@ -679,10 +671,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -695,7 +687,7 @@
     <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -715,8 +707,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="11">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="10">
         <v>10000</v>
       </c>
       <c r="B2" s="5">
@@ -726,15 +718,14 @@
       <c r="D2" s="5">
         <v>0</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="10">
         <v>10000</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="11">
         <v>1666.66</v>
       </c>
-      <c r="H2" s="9"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>672.06</v>
       </c>
@@ -754,7 +745,7 @@
         <v>193.97</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>0</v>
       </c>
@@ -774,7 +765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>0</v>
       </c>
@@ -804,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -881,13 +872,13 @@
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="13">
+      <c r="C2" s="12">
         <v>42005</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="11">
+      <c r="G2" s="10">
         <v>10000</v>
       </c>
       <c r="H2" s="5"/>
@@ -912,7 +903,7 @@
       <c r="B3" s="5">
         <v>31</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="12">
         <v>42036</v>
       </c>
       <c r="D3" s="5"/>
@@ -920,7 +911,7 @@
       <c r="F3" s="5">
         <v>833.33</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="11">
         <v>9166.67</v>
       </c>
       <c r="H3" s="5">
@@ -955,7 +946,7 @@
       <c r="B4" s="5">
         <v>28</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="12">
         <v>42064</v>
       </c>
       <c r="D4" s="5"/>
@@ -963,7 +954,7 @@
       <c r="F4" s="5">
         <v>833.33</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="11">
         <v>8333.34</v>
       </c>
       <c r="H4" s="5">
@@ -998,7 +989,7 @@
       <c r="B5" s="5">
         <v>31</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="12">
         <v>42095</v>
       </c>
       <c r="D5" s="5"/>
@@ -1006,7 +997,7 @@
       <c r="F5" s="5">
         <v>833.33</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="11">
         <v>7500.01</v>
       </c>
       <c r="H5" s="5">
@@ -1041,7 +1032,7 @@
       <c r="B6" s="5">
         <v>30</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="12">
         <v>42125</v>
       </c>
       <c r="D6" s="5"/>
@@ -1049,7 +1040,7 @@
       <c r="F6" s="5">
         <v>833.33</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="11">
         <v>6666.68</v>
       </c>
       <c r="H6" s="5">
@@ -1084,7 +1075,7 @@
       <c r="B7" s="5">
         <v>31</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="12">
         <v>42156</v>
       </c>
       <c r="D7" s="5"/>
@@ -1092,7 +1083,7 @@
       <c r="F7" s="5">
         <v>833.33</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="11">
         <v>5833.35</v>
       </c>
       <c r="H7" s="5">
@@ -1127,7 +1118,7 @@
       <c r="B8" s="5">
         <v>30</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="12">
         <v>42186</v>
       </c>
       <c r="D8" s="5"/>
@@ -1135,7 +1126,7 @@
       <c r="F8" s="5">
         <v>833.33</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="11">
         <v>5000.0200000000004</v>
       </c>
       <c r="H8" s="5">
@@ -1170,7 +1161,7 @@
       <c r="B9" s="5">
         <v>31</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="12">
         <v>42217</v>
       </c>
       <c r="D9" s="5"/>
@@ -1178,7 +1169,7 @@
       <c r="F9" s="5">
         <v>833.33</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="11">
         <v>4166.6899999999996</v>
       </c>
       <c r="H9" s="5">
@@ -1213,7 +1204,7 @@
       <c r="B10" s="5">
         <v>31</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="12">
         <v>42248</v>
       </c>
       <c r="D10" s="5"/>
@@ -1221,7 +1212,7 @@
       <c r="F10" s="5">
         <v>833.33</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="11">
         <v>3333.36</v>
       </c>
       <c r="H10" s="5">
@@ -1256,7 +1247,7 @@
       <c r="B11" s="5">
         <v>30</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="12">
         <v>42278</v>
       </c>
       <c r="D11" s="5"/>
@@ -1264,7 +1255,7 @@
       <c r="F11" s="5">
         <v>833.33</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="11">
         <v>2500.0300000000002</v>
       </c>
       <c r="H11" s="5">
@@ -1299,7 +1290,7 @@
       <c r="B12" s="5">
         <v>31</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="12">
         <v>42309</v>
       </c>
       <c r="D12" s="5"/>
@@ -1307,7 +1298,7 @@
       <c r="F12" s="5">
         <v>833.33</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="11">
         <v>1666.7</v>
       </c>
       <c r="H12" s="5">
@@ -1342,7 +1333,7 @@
       <c r="B13" s="5">
         <v>30</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="12">
         <v>42339</v>
       </c>
       <c r="D13" s="5"/>
@@ -1385,7 +1376,7 @@
       <c r="B14" s="5">
         <v>31</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="12">
         <v>42370</v>
       </c>
       <c r="D14" s="5"/>

</xml_diff>